<commit_message>
reads csv's into clean_data adds descriptions to metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_survey_locations_metadata.xlsx
+++ b/data-raw/metadata/feather_survey_locations_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD6AEF3-123D-4E31-BE60-2EDE29F4EB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53032E2-57BE-4109-AB1B-0EDD20F5E724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27090" yWindow="1710" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25620" yWindow="1440" windowWidth="22230" windowHeight="13035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -91,64 +91,7 @@
     <t>attribute_name</t>
   </si>
   <si>
-    <t xml:space="preserve">survey_id           </t>
-  </si>
-  <si>
     <t>date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flow       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">turbidity            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">temperature          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">start_time          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">end_time             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">section_name        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">units_covered        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">unit                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">count                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">size_class           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">est_size             </t>
-  </si>
-  <si>
-    <t xml:space="preserve">substrate            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">instream_cover      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">overhead_cover       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">water_depth_m        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">run                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tagged           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">clipped  </t>
   </si>
   <si>
     <t>Flow in cfs</t>
@@ -157,70 +100,10 @@
     <t>interval</t>
   </si>
   <si>
-    <t xml:space="preserve">Temperature of Water </t>
-  </si>
-  <si>
-    <t xml:space="preserve">celsius </t>
-  </si>
-  <si>
     <t>Date snorkel data was collected</t>
   </si>
   <si>
-    <t>Turbidity measured at survey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substrate description from survey location </t>
-  </si>
-  <si>
-    <t>Time when snorkel survey started</t>
-  </si>
-  <si>
-    <t>Number of fish observed</t>
-  </si>
-  <si>
-    <t>whole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instream cover at survey location </t>
-  </si>
-  <si>
-    <t>Overhead cover at survey location</t>
-  </si>
-  <si>
-    <t>Depth on water in meters</t>
-  </si>
-  <si>
-    <t>Location were snorkel data was collected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weather      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">hydrology    </t>
-  </si>
-  <si>
     <t>location</t>
-  </si>
-  <si>
-    <t>survey_type</t>
-  </si>
-  <si>
-    <t>section_type</t>
-  </si>
-  <si>
-    <t>species</t>
-  </si>
-  <si>
-    <t>fork_length</t>
-  </si>
-  <si>
-    <t>bank_distance</t>
-  </si>
-  <si>
-    <t>unit_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">visibility </t>
   </si>
   <si>
     <t>section_number</t>
@@ -229,37 +112,10 @@
     <t>dateTime</t>
   </si>
   <si>
-    <t>Fork length of juvenile</t>
-  </si>
-  <si>
-    <t>millimeter</t>
-  </si>
-  <si>
-    <t>Distance from the bank</t>
-  </si>
-  <si>
-    <t>meter</t>
-  </si>
-  <si>
-    <t>Identification number of survey</t>
-  </si>
-  <si>
-    <t>Number of map section from DMP</t>
-  </si>
-  <si>
     <t>ordinal</t>
   </si>
   <si>
     <t>cubicFeetPerSecond</t>
-  </si>
-  <si>
-    <t>unsure</t>
-  </si>
-  <si>
-    <t>count of fish</t>
-  </si>
-  <si>
-    <t>integer</t>
   </si>
   <si>
     <t>YYYY-MM-DD</t>
@@ -268,41 +124,67 @@
     <t>enumerated</t>
   </si>
   <si>
-    <t>Fish size classification. Levels = c("III" "I"   NA    "II"  "VI"  "IV"  "V"   "VII")</t>
-  </si>
-  <si>
-    <t>hh:mm:ss</t>
-  </si>
-  <si>
     <t>survey_id</t>
   </si>
   <si>
     <t>Feather River Snorkel Survey</t>
   </si>
   <si>
-    <t>NTU</t>
+    <t>river_mile</t>
   </si>
   <si>
-    <t>Location were snorkel data was collected. Levels = c(Hatchery Riffle, G95, Mo's Ditch, 
-Bedrock Park Riffle, Trailer Park Riffle, Aleck Riffle, Steep Riffle, Eye Riffle, Big Riffle, Vance Riffle, McFarland, Junkyard Riffle, Gateway Riffle, Hatchery Ditch, Matthews Riffle, Gridley Riffle, Robinson Riffle, Kiester Riffle, Goose Riffle, Hatchery and Mo's Riffles, Auditorium Riffle, Hatchery Ditch and Mo's Ditch)</t>
+    <t xml:space="preserve">gps_coordinate </t>
   </si>
   <si>
-    <t>Weather conditions when data was collected. Levels = c(clear, sunny, clear and windy, cloudy, partly cloudy, precipitation, hazy, windy, clear and hot, overcast)</t>
+    <t>location_table_id</t>
   </si>
   <si>
-    <t>Features of stream. Levels = c(riffle, glide, glide edgewater, riffle edgewater, backwater, pool)</t>
+    <t>water_temp</t>
   </si>
   <si>
-    <t>Run type of the fish counted. Levels = c(unknown, spring, fall, late fall)</t>
+    <t>weather</t>
   </si>
   <si>
-    <t>If fish was tagged or not. Levels = c(TRUE, FALSE)</t>
+    <t>flow</t>
   </si>
   <si>
-    <t>If fish fin is clipped. Levels = c(TRUE, FALSE)</t>
+    <t>number_of_divers</t>
   </si>
   <si>
-    <t>Fish species. Levels = c(chinook, unknown)</t>
+    <t>reach_length</t>
+  </si>
+  <si>
+    <t>reach_width</t>
+  </si>
+  <si>
+    <t>channel_width</t>
+  </si>
+  <si>
+    <t>channel_type</t>
+  </si>
+  <si>
+    <t>snorkel_survey</t>
+  </si>
+  <si>
+    <t>Identification number of survey location table</t>
+  </si>
+  <si>
+    <t>mini-snorkel-survey</t>
+  </si>
+  <si>
+    <t>Temperature of water in degrees Fahrenheit</t>
+  </si>
+  <si>
+    <t>fahrenheit</t>
+  </si>
+  <si>
+    <t>Number of divers during mini-snorkel survey</t>
+  </si>
+  <si>
+    <t>Feather channel where survey was conducted. Levels = c("Mainchannel", "Mainchannel Branch", "Sidechannel")</t>
+  </si>
+  <si>
+    <t>Location were mini snorkel data was collected. Levels = c("aleck riffle", "hatchery ditch", hour bars"</t>
   </si>
 </sst>
 </file>
@@ -374,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -409,9 +291,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -641,8 +520,8 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -717,17 +596,19 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="3"/>
@@ -753,31 +634,33 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="2"/>
       <c r="J3" s="5" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="K3" s="6"/>
-      <c r="L3" s="17">
-        <v>36259</v>
+      <c r="L3" s="16">
+        <v>36963</v>
       </c>
-      <c r="M3" s="17">
-        <v>44099</v>
+      <c r="M3" s="16">
+        <v>37125</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -795,36 +678,26 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="10"/>
-      <c r="L4" s="11">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>9564</v>
-      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="3"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -841,26 +714,38 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="F5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="5"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="3"/>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>69</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -877,36 +762,20 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="1"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="2"/>
       <c r="J6" s="5"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="13">
-        <v>0</v>
-      </c>
-      <c r="M6" s="13">
-        <v>4</v>
-      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -923,35 +792,23 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="1"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="2"/>
       <c r="J7" s="5"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="16">
-        <v>0</v>
+      <c r="L7" s="11">
+        <v>46</v>
       </c>
       <c r="M7" s="3">
-        <v>21.67</v>
+        <v>66</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -969,32 +826,32 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>48</v>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="F8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="5" t="s">
-        <v>81</v>
-      </c>
+      <c r="J8" s="5"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="18">
-        <v>4.8611111111111112E-2</v>
-      </c>
-      <c r="M8" s="18">
-        <v>0.98611111111111116</v>
-      </c>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -1011,32 +868,26 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="5" t="s">
-        <v>81</v>
-      </c>
+      <c r="J9" s="5"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="18">
-        <v>5.0694444444444445E-2</v>
-      </c>
-      <c r="M9" s="18">
-        <v>0.66111111111111109</v>
-      </c>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -1053,18 +904,12 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1089,18 +934,12 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1125,18 +964,12 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1161,36 +994,26 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="3"/>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="11">
-        <v>0</v>
-      </c>
-      <c r="M13" s="15">
-        <v>30000</v>
-      </c>
+      <c r="L13" s="11"/>
+      <c r="M13" s="15"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1207,18 +1030,12 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1242,37 +1059,19 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A15" s="12"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="2"/>
       <c r="J15" s="3"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="15">
-        <v>950</v>
-      </c>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1288,19 +1087,11 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A16" s="12"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="1"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1324,19 +1115,11 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A17" s="12"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="1"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1360,19 +1143,11 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1396,37 +1171,19 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A19" s="12"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="1"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
       <c r="I19" s="2"/>
       <c r="J19" s="3"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="M19" s="13">
-        <v>5</v>
-      </c>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1442,19 +1199,11 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A20" s="12"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="1"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1478,19 +1227,11 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A21" s="12"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E21" s="1"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -1514,19 +1255,11 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A22" s="12"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1550,19 +1283,11 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A23" s="12"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="1"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -1586,19 +1311,11 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="1"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E24" s="1"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1622,19 +1339,11 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A25" s="12"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E25" s="1"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1658,19 +1367,11 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A26" s="12"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E26" s="1"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -1694,19 +1395,11 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A27" s="12"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E27" s="1"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -1730,37 +1423,19 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="1"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="3"/>
       <c r="I28" s="2"/>
       <c r="J28" s="3"/>
       <c r="K28" s="2"/>
-      <c r="L28" s="3">
-        <v>0</v>
-      </c>
-      <c r="M28" s="3">
-        <v>900</v>
-      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -1776,37 +1451,19 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A29" s="12"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="1"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
       <c r="I29" s="2"/>
       <c r="J29" s="3"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="14">
-        <v>0</v>
-      </c>
-      <c r="M29" s="14">
-        <v>10</v>
-      </c>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -1822,19 +1479,11 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A30" s="12"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="E30" s="1"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -1858,37 +1507,19 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A31" s="12"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
       <c r="I31" s="2"/>
       <c r="J31" s="3"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="M31" s="14">
-        <v>9</v>
-      </c>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -1904,19 +1535,11 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="A32" s="12"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="1"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E32" s="1"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -29144,16 +28767,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C63:C1006 C39:C51 C1:C32 C35:C37" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C63:C1006 C39:C51 C35:C37 C1:C32" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E39:E1006 E1:E32 E35:E37" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E39:E1006 E35:E37 E1:E32" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F39:F1006 F1:F32 F35:F37" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F39:F1006 F35:F37 F1:F32" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H39:H1006 H1:H32 H35:H37" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H39:H1006 H35:H37 H1:H32" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -29217,10 +28840,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -29251,10 +28874,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>65</v>
+      <c r="C3" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>

</xml_diff>

<commit_message>
drafts survey_loc metadata, adds TODOs and questions
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_survey_locations_metadata.xlsx
+++ b/data-raw/metadata/feather_survey_locations_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53032E2-57BE-4109-AB1B-0EDD20F5E724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40C8012-C82C-4BC8-B152-C330CCED576A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25620" yWindow="1440" windowWidth="22230" windowHeight="13035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -163,9 +163,6 @@
     <t>channel_type</t>
   </si>
   <si>
-    <t>snorkel_survey</t>
-  </si>
-  <si>
     <t>Identification number of survey location table</t>
   </si>
   <si>
@@ -185,6 +182,18 @@
   </si>
   <si>
     <t>Location were mini snorkel data was collected. Levels = c("aleck riffle", "hatchery ditch", hour bars"</t>
+  </si>
+  <si>
+    <t>Weather conditions during survey. Levels - c("Direct Sunlight", "Overcast")</t>
+  </si>
+  <si>
+    <t>Latitude and longitude of survey location</t>
+  </si>
+  <si>
+    <t>River mile where survey was conducted</t>
+  </si>
+  <si>
+    <t>Width of channel in feet</t>
   </si>
 </sst>
 </file>
@@ -256,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -301,6 +310,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -520,8 +532,8 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -599,13 +611,13 @@
         <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>31</v>
@@ -643,7 +655,7 @@
         <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>27</v>
@@ -681,12 +693,14 @@
         <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
@@ -717,13 +731,13 @@
         <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
@@ -732,7 +746,7 @@
         <v>23</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>17</v>
@@ -764,10 +778,18 @@
       <c r="A6" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="1"/>
+      <c r="B6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -794,9 +816,13 @@
       <c r="A7" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="5"/>
       <c r="G7" s="3"/>
@@ -834,7 +860,9 @@
       <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
@@ -871,12 +899,14 @@
         <v>40</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
@@ -908,16 +938,24 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="2"/>
       <c r="J10" s="5"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="3"/>
+      <c r="L10" s="19">
+        <v>25</v>
+      </c>
+      <c r="M10" s="19">
+        <v>25</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -938,16 +976,24 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="2"/>
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="3"/>
+      <c r="L11" s="19">
+        <v>0</v>
+      </c>
+      <c r="M11" s="19">
+        <v>160</v>
+      </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -966,18 +1012,28 @@
       <c r="A12" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="2"/>
       <c r="J12" s="5"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="3"/>
+      <c r="L12" s="11">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>160</v>
+      </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -997,12 +1053,14 @@
         <v>44</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1032,10 +1090,18 @@
       <c r="A14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>

</xml_diff>

<commit_message>
finish drafting survey_location metadata, adds questions to md
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_survey_locations_metadata.xlsx
+++ b/data-raw/metadata/feather_survey_locations_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40C8012-C82C-4BC8-B152-C330CCED576A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6750C254-5F3E-4D81-878D-C7017615B86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -195,6 +195,12 @@
   <si>
     <t>Width of channel in feet</t>
   </si>
+  <si>
+    <t>Survey reach length</t>
+  </si>
+  <si>
+    <t>Survey reach width</t>
+  </si>
 </sst>
 </file>
 
@@ -265,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -303,9 +309,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="21" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -532,8 +535,8 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -754,10 +757,10 @@
       <c r="I5" s="2"/>
       <c r="J5" s="5"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="7">
+      <c r="L5" s="18">
         <v>0</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="18">
         <v>69</v>
       </c>
       <c r="N5" s="1"/>
@@ -819,22 +822,26 @@
       <c r="B7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="F7" s="5"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="2"/>
       <c r="J7" s="5"/>
       <c r="K7" s="6"/>
-      <c r="L7" s="11">
+      <c r="L7" s="15">
         <v>46</v>
       </c>
-      <c r="M7" s="3">
-        <v>66</v>
+      <c r="M7" s="15">
+        <v>66.599999999999994</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -878,8 +885,12 @@
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
+      <c r="L8" s="18">
+        <v>0</v>
+      </c>
+      <c r="M8" s="18">
+        <v>2000</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -916,8 +927,12 @@
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
+      <c r="L9" s="18">
+        <v>1</v>
+      </c>
+      <c r="M9" s="18">
+        <v>3</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -936,24 +951,32 @@
       <c r="A10" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I10" s="2"/>
       <c r="J10" s="5"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="19">
+      <c r="L10" s="3">
         <v>25</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="3">
         <v>25</v>
       </c>
       <c r="N10" s="1"/>
@@ -974,25 +997,33 @@
       <c r="A11" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I11" s="2"/>
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="19">
-        <v>0</v>
+      <c r="L11" s="3">
+        <v>4</v>
       </c>
-      <c r="M11" s="19">
-        <v>160</v>
+      <c r="M11" s="3">
+        <v>4</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1015,16 +1046,22 @@
       <c r="B12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="I12" s="2"/>
       <c r="J12" s="5"/>
       <c r="K12" s="6"/>
@@ -28942,7 +28979,7 @@
       <c r="B3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="9"/>

</xml_diff>

<commit_message>
modifies location_table_id, validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_survey_locations_metadata.xlsx
+++ b/data-raw/metadata/feather_survey_locations_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-mini-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D4FB88-3179-4B1E-95D8-895C15888F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1099CD9A-321A-4113-901B-F5BC0D5EDEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1580" yWindow="1190" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="60">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>Feather channel where survey was conducted. Levels = c("mainchannel", "mainchannel branch", "sidechannel")</t>
+  </si>
+  <si>
+    <t>whole</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -533,7 +539,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -614,7 +620,7 @@
         <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>42</v>
@@ -622,14 +628,24 @@
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="I2" s="2"/>
       <c r="J2" s="5"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
+      <c r="L2" s="3">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3">
+        <v>146</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>

</xml_diff>